<commit_message>
Feat: make the backend for import feature
</commit_message>
<xml_diff>
--- a/public/templates/questions-template.xlsx
+++ b/public/templates/questions-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT DEPT\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BDAC8B-80C4-4446-A394-9DEF91B48B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73D6890-83F1-4686-8385-350B8676644F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{801E68DC-DC19-4572-8C27-D9A09CFF2400}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Type</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>long</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Correct Option</t>
   </si>
 </sst>
 </file>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A38FFC-8A68-48F3-BF68-9E791559A789}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,9 +528,10 @@
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,8 +568,11 @@
       <c r="L1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -593,8 +603,11 @@
       <c r="J2" t="s">
         <v>19</v>
       </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -614,7 +627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>

</xml_diff>